<commit_message>
- rev 4a prod boards are finished, created BOM & gerbers
</commit_message>
<xml_diff>
--- a/eagle design/MJ808 clone - all driver - POC - BOM.xlsx
+++ b/eagle design/MJ808 clone - all driver - POC - BOM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="15" windowWidth="16125" windowHeight="6465"/>
+    <workbookView xWindow="1335" yWindow="2040" windowWidth="16125" windowHeight="6465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MJ808 clone - all driver- POC" sheetId="4" r:id="rId1"/>
+    <sheet name="MJ808 clone - all driver- prod" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="167">
   <si>
     <t>Value</t>
   </si>
@@ -425,19 +426,117 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>0.1ÎĽF</t>
+  </si>
+  <si>
+    <t>81-GRM022R61A104ME1L</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Murata-Electronics/GRM022R61A104ME01L?qs=5aG0NVq1C4wp%2FlR6SQtdFw%3D%3D</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R8, R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-RCS040210K0FKED </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Vishay-Dale/RCS040210K0FKED?qs=sGAEpiMZZMvdGkrng054t9clqp6gtJJdXBtFSxkAevBVVwivOSsTiw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-CRCW0805120RFKEAH </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Vishay-Dale/CRCW0805120RFKEAHP?qs=40TFAHZMFvctVwM59SMR3Q%3D%3D</t>
+  </si>
+  <si>
+    <t>1ÎĽF</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-GRM155C81E105ME1J </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Murata-Electronics/GRM155C81E105ME11J?qs=sGAEpiMZZMs0AnBnWHyRQN7%2FAA2D2lPPOf3fPa9BEu8yEyQEE4mRxQ%3D%3D</t>
+  </si>
+  <si>
+    <t>1ÎĽF / 10V</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>ICSP</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Molex/503480-0600?qs=sGAEpiMZZMs7i6cT6ogu42UM2hUx5mbP%252B%2F1j744pfik%3D</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/CTS-Electronic-Components/741X083331JP?qs=%2Fha2pyFadujD8YpjBW%252BfQlaV1dM%2FInzfSJj4DoCaKLvSeOdACTDR1g%3D%3D</t>
+  </si>
+  <si>
+    <t>LDK320SOT-23-5L</t>
+  </si>
+  <si>
+    <t>SOT-23-5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-LDK320M50R </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/STMicroelectronics/LDK320M50R?qs=sGAEpiMZZMsGz1a6aV8DcGP3s75Ab7uy10GFwtAx4R4%3D</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>TL3305-844809</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">612-TL3305CF260QG </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/E-Switch/TL3305CF260QG?qs=sGAEpiMZZMsgGjVA3toVBKeJCRa1nG8XQ7LDZe51kyo%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71-WSLT2010R2500FEB1 </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Vishay-Dale/WSLT2010R2500FEB18?qs=sGAEpiMZZMtlleCFQhR%2FzfECrHCYVtmG4D4SV6Ab70w%3D</t>
+  </si>
+  <si>
+    <t>0.25 / 1W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -615,6 +714,143 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -914,122 +1150,294 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="85" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="85"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="127">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1 2" xfId="104"/>
+    <cellStyle name="20% - Accent1 3" xfId="62"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2 2" xfId="108"/>
+    <cellStyle name="20% - Accent2 3" xfId="66"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3 2" xfId="112"/>
+    <cellStyle name="20% - Accent3 3" xfId="70"/>
     <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4 2" xfId="116"/>
+    <cellStyle name="20% - Accent4 3" xfId="74"/>
     <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5 2" xfId="120"/>
+    <cellStyle name="20% - Accent5 3" xfId="78"/>
     <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6 2" xfId="124"/>
+    <cellStyle name="20% - Accent6 3" xfId="82"/>
     <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1 2" xfId="105"/>
+    <cellStyle name="40% - Accent1 3" xfId="63"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2 2" xfId="109"/>
+    <cellStyle name="40% - Accent2 3" xfId="67"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3 2" xfId="113"/>
+    <cellStyle name="40% - Accent3 3" xfId="71"/>
     <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4 2" xfId="117"/>
+    <cellStyle name="40% - Accent4 3" xfId="75"/>
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5 2" xfId="121"/>
+    <cellStyle name="40% - Accent5 3" xfId="79"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6 2" xfId="125"/>
+    <cellStyle name="40% - Accent6 3" xfId="83"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1 2" xfId="106"/>
+    <cellStyle name="60% - Accent1 3" xfId="64"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2 2" xfId="110"/>
+    <cellStyle name="60% - Accent2 3" xfId="68"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3 2" xfId="114"/>
+    <cellStyle name="60% - Accent3 3" xfId="72"/>
     <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4 2" xfId="118"/>
+    <cellStyle name="60% - Accent4 3" xfId="76"/>
     <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5 2" xfId="122"/>
+    <cellStyle name="60% - Accent5 3" xfId="80"/>
     <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6 2" xfId="126"/>
+    <cellStyle name="60% - Accent6 3" xfId="84"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent1 2" xfId="103"/>
+    <cellStyle name="Accent1 3" xfId="61"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent2 2" xfId="107"/>
+    <cellStyle name="Accent2 3" xfId="65"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent3 2" xfId="111"/>
+    <cellStyle name="Accent3 3" xfId="69"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent4 2" xfId="115"/>
+    <cellStyle name="Accent4 3" xfId="73"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent5 2" xfId="119"/>
+    <cellStyle name="Accent5 3" xfId="77"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Accent6 2" xfId="123"/>
+    <cellStyle name="Accent6 3" xfId="81"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Bad 2" xfId="92"/>
+    <cellStyle name="Bad 3" xfId="50"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Calculation 2" xfId="96"/>
+    <cellStyle name="Calculation 3" xfId="54"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Check Cell 2" xfId="98"/>
+    <cellStyle name="Check Cell 3" xfId="56"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text 2" xfId="101"/>
+    <cellStyle name="Explanatory Text 3" xfId="59"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Good 2" xfId="91"/>
+    <cellStyle name="Good 3" xfId="49"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 1 2" xfId="87"/>
+    <cellStyle name="Heading 1 3" xfId="45"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 2 2" xfId="88"/>
+    <cellStyle name="Heading 2 3" xfId="46"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 3 2" xfId="89"/>
+    <cellStyle name="Heading 3 3" xfId="47"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Heading 4 2" xfId="90"/>
+    <cellStyle name="Heading 4 3" xfId="48"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Input 2" xfId="94"/>
+    <cellStyle name="Input 3" xfId="52"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Linked Cell 2" xfId="97"/>
+    <cellStyle name="Linked Cell 3" xfId="55"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="93"/>
+    <cellStyle name="Neutral 3" xfId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="85"/>
+    <cellStyle name="Normal 3" xfId="43"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note 2" xfId="100"/>
+    <cellStyle name="Note 3" xfId="58"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Output 2" xfId="95"/>
+    <cellStyle name="Output 3" xfId="53"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title 2" xfId="86"/>
+    <cellStyle name="Title 3" xfId="44"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Total 2" xfId="102"/>
+    <cellStyle name="Total 3" xfId="60"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Warning Text 2" xfId="99"/>
+    <cellStyle name="Warning Text 3" xfId="57"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1320,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2001,4 +2409,535 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="11">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="11">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="11">
+        <v>120</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="11">
+        <v>1</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="11">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5034800600</v>
+      </c>
+      <c r="C8" s="11">
+        <v>5034800600</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="11">
+        <v>402</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="11">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="11">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="11">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="11">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="11">
+        <v>1</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="11">
+        <v>1</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H12" r:id="rId1"/>
+    <hyperlink ref="H13" r:id="rId2"/>
+    <hyperlink ref="H14" r:id="rId3"/>
+    <hyperlink ref="H15" r:id="rId4"/>
+    <hyperlink ref="H17" r:id="rId5"/>
+    <hyperlink ref="H18" r:id="rId6"/>
+    <hyperlink ref="H20" r:id="rId7"/>
+    <hyperlink ref="H10" r:id="rId8"/>
+    <hyperlink ref="H9" r:id="rId9"/>
+    <hyperlink ref="H8" r:id="rId10"/>
+    <hyperlink ref="H19" r:id="rId11"/>
+    <hyperlink ref="H4" r:id="rId12"/>
+    <hyperlink ref="H5" r:id="rId13"/>
+    <hyperlink ref="H3" r:id="rId14"/>
+    <hyperlink ref="H2" r:id="rId15"/>
+    <hyperlink ref="H7" r:id="rId16"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>